<commit_message>
Updating the repo for publication
</commit_message>
<xml_diff>
--- a/Jones_urchin_manuscript/03_clean_data/species_categories_with_common_names.xlsx
+++ b/Jones_urchin_manuscript/03_clean_data/species_categories_with_common_names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecjones/Documents/GitHub/Alec_Jones_Urchin_manuscript/Jones_urchin_manuscript/03_clean_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CF7B8D-AFB1-A44D-9C55-522B04A89B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192E78F2-8B60-7847-A808-1493057DE83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32460" windowHeight="19280" xr2:uid="{D2BA59DC-45B7-294E-A164-CA2813AED3D9}"/>
   </bookViews>

</xml_diff>